<commit_message>
Beispieldatensatz aktualisieren und Rahmenlinien für Filterkriterien hinzufügen, Tabellenlayout updaten
</commit_message>
<xml_diff>
--- a/Beispieldaten/Beispieldaten.xlsx
+++ b/Beispieldaten/Beispieldaten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Webtechnologie_23_24\Beispieldaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014DF01B-5E30-498F-B701-937C746D5B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED352BB0-5D1C-4343-B623-3E2F552B9BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AABB9DB3-64DF-4BA6-A818-950DF034666B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{AABB9DB3-64DF-4BA6-A818-950DF034666B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Kundenliste!$A$4:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$Q$411</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$Q$423</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CBA60F-BA56-404D-B045-95D79F60DCCF}">
   <dimension ref="A1:Q423"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D389" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L405" sqref="L405:L406"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G390" sqref="G390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21014,7 +21014,7 @@
         <v>28</v>
       </c>
       <c r="G382">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H382" t="s">
         <v>30</v>
@@ -21067,7 +21067,7 @@
         <v>28</v>
       </c>
       <c r="G383">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H383" t="s">
         <v>30</v>
@@ -21120,7 +21120,7 @@
         <v>28</v>
       </c>
       <c r="G384">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H384" t="s">
         <v>30</v>
@@ -21173,7 +21173,7 @@
         <v>28</v>
       </c>
       <c r="G385">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H385" t="s">
         <v>30</v>
@@ -21226,7 +21226,7 @@
         <v>28</v>
       </c>
       <c r="G386">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H386" t="s">
         <v>30</v>
@@ -21279,7 +21279,7 @@
         <v>28</v>
       </c>
       <c r="G387">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H387" t="s">
         <v>30</v>
@@ -21332,7 +21332,7 @@
         <v>28</v>
       </c>
       <c r="G388">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H388" t="s">
         <v>30</v>
@@ -21385,7 +21385,7 @@
         <v>28</v>
       </c>
       <c r="G389">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H389" t="s">
         <v>30</v>
@@ -21438,7 +21438,7 @@
         <v>28</v>
       </c>
       <c r="G390">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H390" t="s">
         <v>30</v>
@@ -21491,7 +21491,7 @@
         <v>28</v>
       </c>
       <c r="G391">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H391" t="s">
         <v>30</v>
@@ -21544,7 +21544,7 @@
         <v>28</v>
       </c>
       <c r="G392">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H392" t="s">
         <v>30</v>
@@ -21597,7 +21597,7 @@
         <v>28</v>
       </c>
       <c r="G393">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H393" t="s">
         <v>30</v>
@@ -21650,7 +21650,7 @@
         <v>28</v>
       </c>
       <c r="G394">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H394" t="s">
         <v>30</v>
@@ -21703,7 +21703,7 @@
         <v>28</v>
       </c>
       <c r="G395">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H395" t="s">
         <v>30</v>
@@ -21756,7 +21756,7 @@
         <v>28</v>
       </c>
       <c r="G396">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H396" t="s">
         <v>30</v>
@@ -21809,7 +21809,7 @@
         <v>28</v>
       </c>
       <c r="G397">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H397" t="s">
         <v>30</v>
@@ -21862,7 +21862,7 @@
         <v>28</v>
       </c>
       <c r="G398">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H398" t="s">
         <v>30</v>
@@ -21915,7 +21915,7 @@
         <v>28</v>
       </c>
       <c r="G399">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H399" t="s">
         <v>30</v>
@@ -21968,7 +21968,7 @@
         <v>28</v>
       </c>
       <c r="G400">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H400" t="s">
         <v>30</v>
@@ -22021,7 +22021,7 @@
         <v>28</v>
       </c>
       <c r="G401">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H401" t="s">
         <v>30</v>
@@ -22074,7 +22074,7 @@
         <v>28</v>
       </c>
       <c r="G402">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H402" t="s">
         <v>30</v>
@@ -22127,7 +22127,7 @@
         <v>28</v>
       </c>
       <c r="G403">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H403" t="s">
         <v>30</v>
@@ -22180,7 +22180,7 @@
         <v>28</v>
       </c>
       <c r="G404">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H404" t="s">
         <v>30</v>
@@ -22233,7 +22233,7 @@
         <v>28</v>
       </c>
       <c r="G405">
-        <v>87654321</v>
+        <v>98743245</v>
       </c>
       <c r="H405" t="s">
         <v>30</v>
@@ -23167,7 +23167,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q411" xr:uid="{B5CBA60F-BA56-404D-B045-95D79F60DCCF}"/>
+  <autoFilter ref="A1:Q423" xr:uid="{B5CBA60F-BA56-404D-B045-95D79F60DCCF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q405">
     <sortCondition ref="A2:A405"/>
     <sortCondition ref="C2:C405"/>

</xml_diff>

<commit_message>
Streamlit-Server Diagramme und Excel-Datei updaten
</commit_message>
<xml_diff>
--- a/Beispieldaten/Beispieldaten.xlsx
+++ b/Beispieldaten/Beispieldaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Webtechnologie_23_24\Beispieldaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED352BB0-5D1C-4343-B623-3E2F552B9BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA72D53-84B4-4233-8BB3-679E85145849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{AABB9DB3-64DF-4BA6-A818-950DF034666B}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3526" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3526" uniqueCount="124">
   <si>
     <t>Isocyanate</t>
   </si>
@@ -405,6 +405,15 @@
   </si>
   <si>
     <t>Special Solutions Ltd.</t>
+  </si>
+  <si>
+    <t>Sahara Polymer Innovations</t>
+  </si>
+  <si>
+    <t>RapidRise Polymer Africa Ltd.</t>
+  </si>
+  <si>
+    <t>EcoTech Polymers Asia</t>
   </si>
 </sst>
 </file>
@@ -779,26 +788,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CBA60F-BA56-404D-B045-95D79F60DCCF}">
   <dimension ref="A1:Q423"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G390" sqref="G390"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1210,7 +1222,7 @@
         <v>200123</v>
       </c>
       <c r="M8" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N8">
         <v>2019</v>
@@ -1263,7 +1275,7 @@
         <v>235678</v>
       </c>
       <c r="M9" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N9">
         <v>2019</v>
@@ -2323,7 +2335,7 @@
         <v>200123</v>
       </c>
       <c r="M29" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N29">
         <v>2022</v>
@@ -2429,7 +2441,7 @@
         <v>215678</v>
       </c>
       <c r="M31" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N31">
         <v>2023</v>
@@ -3171,7 +3183,7 @@
         <v>200123</v>
       </c>
       <c r="M45" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N45">
         <v>2019</v>
@@ -3224,7 +3236,7 @@
         <v>200123</v>
       </c>
       <c r="M46" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N46">
         <v>2020</v>
@@ -3277,7 +3289,7 @@
         <v>200123</v>
       </c>
       <c r="M47" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N47">
         <v>2022</v>
@@ -3436,7 +3448,7 @@
         <v>215678</v>
       </c>
       <c r="M50" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N50">
         <v>2018</v>
@@ -4602,7 +4614,7 @@
         <v>215678</v>
       </c>
       <c r="M72" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N72">
         <v>2019</v>
@@ -4655,7 +4667,7 @@
         <v>235678</v>
       </c>
       <c r="M73" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N73">
         <v>2020</v>
@@ -5609,7 +5621,7 @@
         <v>215678</v>
       </c>
       <c r="M91" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N91">
         <v>2022</v>
@@ -5662,7 +5674,7 @@
         <v>235678</v>
       </c>
       <c r="M92" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N92">
         <v>2020</v>
@@ -7040,7 +7052,7 @@
         <v>200123</v>
       </c>
       <c r="M118" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N118">
         <v>2020</v>
@@ -7093,7 +7105,7 @@
         <v>200123</v>
       </c>
       <c r="M119" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N119">
         <v>2022</v>
@@ -8842,7 +8854,7 @@
         <v>235678</v>
       </c>
       <c r="M152" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N152">
         <v>2021</v>
@@ -10167,7 +10179,7 @@
         <v>200123</v>
       </c>
       <c r="M177" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N177">
         <v>2022</v>
@@ -10273,7 +10285,7 @@
         <v>215678</v>
       </c>
       <c r="M179" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N179">
         <v>2023</v>
@@ -10432,7 +10444,7 @@
         <v>235678</v>
       </c>
       <c r="M182" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N182">
         <v>2019</v>
@@ -11598,7 +11610,7 @@
         <v>200123</v>
       </c>
       <c r="M204" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N204">
         <v>2019</v>
@@ -11757,7 +11769,7 @@
         <v>235678</v>
       </c>
       <c r="M207" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N207">
         <v>2023</v>
@@ -12817,7 +12829,7 @@
         <v>200123</v>
       </c>
       <c r="M227" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N227">
         <v>2022</v>
@@ -12923,7 +12935,7 @@
         <v>215678</v>
       </c>
       <c r="M229" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N229">
         <v>2019</v>
@@ -14036,7 +14048,7 @@
         <v>200123</v>
       </c>
       <c r="M250" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N250">
         <v>2018</v>
@@ -14089,7 +14101,7 @@
         <v>200123</v>
       </c>
       <c r="M251" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N251">
         <v>2020</v>
@@ -14354,7 +14366,7 @@
         <v>235678</v>
       </c>
       <c r="M256" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N256">
         <v>2022</v>
@@ -16050,7 +16062,7 @@
         <v>200123</v>
       </c>
       <c r="M288" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N288">
         <v>2022</v>
@@ -16103,7 +16115,7 @@
         <v>200123</v>
       </c>
       <c r="M289" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="N289">
         <v>2023</v>
@@ -16315,7 +16327,7 @@
         <v>215678</v>
       </c>
       <c r="M293" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N293">
         <v>2020</v>
@@ -16368,7 +16380,7 @@
         <v>215678</v>
       </c>
       <c r="M294" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N294">
         <v>2021</v>
@@ -16421,7 +16433,7 @@
         <v>215678</v>
       </c>
       <c r="M295" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N295">
         <v>2023</v>
@@ -18276,7 +18288,7 @@
         <v>215678</v>
       </c>
       <c r="M330" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N330">
         <v>2019</v>
@@ -18329,7 +18341,7 @@
         <v>215678</v>
       </c>
       <c r="M331" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N331">
         <v>2022</v>
@@ -18488,7 +18500,7 @@
         <v>235678</v>
       </c>
       <c r="M334" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N334">
         <v>2020</v>
@@ -18541,7 +18553,7 @@
         <v>235678</v>
       </c>
       <c r="M335" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N335">
         <v>2023</v>
@@ -20131,7 +20143,7 @@
         <v>215678</v>
       </c>
       <c r="M365" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N365">
         <v>2019</v>
@@ -20237,7 +20249,7 @@
         <v>235678</v>
       </c>
       <c r="M367" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N367">
         <v>2020</v>
@@ -21509,7 +21521,7 @@
         <v>215678</v>
       </c>
       <c r="M391" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N391">
         <v>2020</v>
@@ -21562,7 +21574,7 @@
         <v>215678</v>
       </c>
       <c r="M392" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="N392">
         <v>2020</v>

</xml_diff>